<commit_message>
Test case and scenarios
Test case
</commit_message>
<xml_diff>
--- a/Assignment/Module 3/Copy of Scenario of orangehrm.xlsx
+++ b/Assignment/Module 3/Copy of Scenario of orangehrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VishalPC\OneDrive\Desktop\Tops Assignment\jagu-record\Assignment\Module 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E22D4D16-6228-484C-9DC8-64EEBF196A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E5C0C2-BC57-49B6-8CB0-A0DAAE1A206A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="3630" windowWidth="21600" windowHeight="11295" xr2:uid="{BD479DC1-1C6C-4F67-9E37-4DC57FAF22DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BD479DC1-1C6C-4F67-9E37-4DC57FAF22DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -2351,10 +2351,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2656,7 +2652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45826ABD-80DA-4737-829D-D8902C7E661D}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
@@ -4358,8 +4354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317E374A-8E1C-4299-976A-AA1964A85A2F}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C103" sqref="C103:C104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>